<commit_message>
TODO: fix weaviate test
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -1,84 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raydelv/Documents/Code/vdb-comparison/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2443A10-FFF3-514E-B65A-F99AA0F6F8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>VLite2</t>
-  </si>
-  <si>
-    <t>Chroma</t>
-  </si>
-  <si>
-    <t>Pinecone</t>
-  </si>
-  <si>
-    <t>Weaviate</t>
-  </si>
-  <si>
-    <t>Qdrant</t>
-  </si>
-  <si>
-    <t>VLite1</t>
-  </si>
-  <si>
-    <t>Memorize One</t>
-  </si>
-  <si>
-    <t>Remember One</t>
-  </si>
-  <si>
-    <t>Memorize Many</t>
-  </si>
-  <si>
-    <t>Remember Many</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,29 +64,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,126 +442,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VLite1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>VLite2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Chroma</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pinecone</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Weaviate</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Qdrant</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Qdrant</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Pinecone</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1.5322376249823719E-2</v>
-      </c>
-      <c r="C2">
-        <v>1.2484761250671E-2</v>
-      </c>
-      <c r="D2">
-        <v>1.8534155830275269E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.25470818125060762</v>
-      </c>
-      <c r="F2">
-        <v>0.33729569874936721</v>
-      </c>
-      <c r="G2">
-        <v>5.2899849169189113E-2</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Memorize One</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01532237624982372</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.012484761250671</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01853415583027527</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2547081812506076</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3372956987493672</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.05289984916918911</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.05259607249987312</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1581844629102852</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>2.314871957991272E-2</v>
-      </c>
-      <c r="C3">
-        <v>9.254275410203263E-3</v>
-      </c>
-      <c r="D3">
-        <v>1.7598784998990591E-2</v>
-      </c>
-      <c r="E3">
-        <v>0.13242604875005781</v>
-      </c>
-      <c r="F3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Remember One</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.02314871957991272</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.009254275410203263</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01759878499899059</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1324260487500578</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.2710886354208924</v>
       </c>
-      <c r="G3">
-        <v>4.5717626250116147E-2</v>
+      <c r="G3" t="n">
+        <v>0.04571762625011615</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.04762424916960299</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.1175251333403867</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2.6973792079370468E-2</v>
-      </c>
-      <c r="C4">
-        <v>8.1317323331022637E-2</v>
-      </c>
-      <c r="D4">
-        <v>3.0344968204200269</v>
-      </c>
-      <c r="E4">
-        <v>25.741428521249912</v>
-      </c>
-      <c r="F4">
-        <v>1.9927339395892341</v>
-      </c>
-      <c r="G4">
-        <v>0.38673950582975519</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Memorize Many</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.02697379207937047</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.08131732333102264</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.034496820420027</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25.74142852124991</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.992733939589234</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.3867395058297552</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.3717753166600596</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8814553541690111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1.9105057090055201E-2</v>
-      </c>
-      <c r="C5">
-        <v>9.3534379196353254E-3</v>
-      </c>
-      <c r="D5">
-        <v>1.7041967080440371E-2</v>
-      </c>
-      <c r="E5">
-        <v>0.18522626250050961</v>
-      </c>
-      <c r="F5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Remember Many</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0191050570900552</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.009353437919635325</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01704196708044037</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1852262625005096</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.2874525854096282</v>
       </c>
-      <c r="G5">
-        <v>8.3653904589591543E-2</v>
+      <c r="G5" t="n">
+        <v>0.08365390458959154</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0966092412499711</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1196997295890469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new benchmarks after anton input
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raydelv/Documents/Code/vdb-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FFB69D-AB2F-7841-8EBE-043FB49431A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDF4FE3-281E-9840-8FDA-929FB257006B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +82,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -136,11 +141,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,6 +175,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -465,7 +488,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,11 +505,11 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -506,10 +529,10 @@
         <v>1.308769541908987E-2</v>
       </c>
       <c r="D2">
+        <v>1.6154604582116011E-2</v>
+      </c>
+      <c r="E2">
         <v>4.8680750830098977E-2</v>
-      </c>
-      <c r="E2">
-        <v>1.855847166967578E-2</v>
       </c>
       <c r="F2" s="2">
         <v>0.203249946669675</v>
@@ -529,10 +552,10 @@
         <v>1.006178832962178E-2</v>
       </c>
       <c r="D3">
+        <v>1.155560291837901E-2</v>
+      </c>
+      <c r="E3">
         <v>4.4850132090505222E-2</v>
-      </c>
-      <c r="E3">
-        <v>8.7931265409570192E-2</v>
       </c>
       <c r="F3" s="2">
         <v>0.12234464165987451</v>
@@ -552,10 +575,10 @@
         <v>8.2541387079982084E-2</v>
       </c>
       <c r="D4">
+        <v>0.14928332374896849</v>
+      </c>
+      <c r="E4">
         <v>0.37011745250085371</v>
-      </c>
-      <c r="E4">
-        <v>3.0008717458404131</v>
       </c>
       <c r="F4" s="2">
         <v>0.84291694250074212</v>
@@ -575,10 +598,10 @@
         <v>9.7275512502528732E-3</v>
       </c>
       <c r="D5">
+        <v>9.5864124991931025E-3</v>
+      </c>
+      <c r="E5">
         <v>7.9040007500443613E-2</v>
-      </c>
-      <c r="E5">
-        <v>0.1343334045901429</v>
       </c>
       <c r="F5" s="2">
         <v>0.1243101699999534</v>

</xml_diff>